<commit_message>
new names of files + counting the number of people
</commit_message>
<xml_diff>
--- a/Qualität.xlsx
+++ b/Qualität.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martina\Desktop\škola\informatika\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martina\Desktop\škola\informatika\git.projectinf\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>1007000/00012345/Alota Problems</t>
-  </si>
-  <si>
     <t>zaměstnanci</t>
   </si>
   <si>
@@ -39,6 +36,9 @@
   </si>
   <si>
     <t>chyba</t>
+  </si>
+  <si>
+    <t>1007000/00012345/Pan Pes</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -371,21 +371,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>